<commit_message>
Continuacao desenvolvimento do sample V2
Implementação de Persmissons e LocalizationText no NavMenu; Implementação da página de Roles;
</commit_message>
<xml_diff>
--- a/Docs/InsertLocalizationText.xlsx
+++ b/Docs/InsertLocalizationText.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="156">
   <si>
     <t xml:space="preserve">      'en-us'</t>
   </si>
@@ -884,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N294"/>
+  <dimension ref="A1:N310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
-      <selection activeCell="D284" sqref="D284"/>
+    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
+      <selection activeCell="E303" sqref="E303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7861,6 +7861,390 @@
         <v>insert into sysLocalizationText Values(1296,      'en-us','1296','Configs-PageTitle','Configurations',getdate(),getdate())</v>
       </c>
     </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>1297</v>
+      </c>
+      <c r="B295" t="s">
+        <v>0</v>
+      </c>
+      <c r="C295" t="str">
+        <f t="shared" ref="C295" si="29">"'" &amp; A295 &amp; "'"</f>
+        <v>'1297'</v>
+      </c>
+      <c r="D295" t="str">
+        <f>$N$1 &amp; "Logout-Label" &amp; $N$1</f>
+        <v>'Logout-Label'</v>
+      </c>
+      <c r="E295" t="str">
+        <f>$N$1 &amp; "Logout" &amp; $N$1</f>
+        <v>'Logout'</v>
+      </c>
+      <c r="F295" t="str">
+        <f t="shared" ref="F295" si="30">"insert into sysLocalizationText Values(" &amp;A295 &amp; "," &amp; B295 &amp; "," &amp;C295 &amp; "," &amp; D295 &amp; "," &amp; E295 &amp; ",getdate(),getdate())"</f>
+        <v>insert into sysLocalizationText Values(1297,      'en-us','1297','Logout-Label','Logout',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>1298</v>
+      </c>
+      <c r="B296" t="s">
+        <v>0</v>
+      </c>
+      <c r="C296" t="str">
+        <f t="shared" ref="C296" si="31">"'" &amp; A296 &amp; "'"</f>
+        <v>'1298'</v>
+      </c>
+      <c r="D296" t="str">
+        <f>$N$1 &amp; "AlterProfileImage-Description" &amp; $N$1</f>
+        <v>'AlterProfileImage-Description'</v>
+      </c>
+      <c r="E296" t="str">
+        <f>$N$1 &amp; "Drag the file here you wish to upload, or click on buttom above to browse." &amp; $N$1</f>
+        <v>'Drag the file here you wish to upload, or click on buttom above to browse.'</v>
+      </c>
+      <c r="F296" t="str">
+        <f t="shared" ref="F296" si="32">"insert into sysLocalizationText Values(" &amp;A296 &amp; "," &amp; B296 &amp; "," &amp;C296 &amp; "," &amp; D296 &amp; "," &amp; E296 &amp; ",getdate(),getdate())"</f>
+        <v>insert into sysLocalizationText Values(1298,      'en-us','1298','AlterProfileImage-Description','Drag the file here you wish to upload, or click on buttom above to browse.',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>1299</v>
+      </c>
+      <c r="B297" t="s">
+        <v>0</v>
+      </c>
+      <c r="C297" t="str">
+        <f t="shared" ref="C297:C310" si="33">"'" &amp; A297 &amp; "'"</f>
+        <v>'1299'</v>
+      </c>
+      <c r="D297" t="str">
+        <f>$N$1 &amp; "Menu-Superadmin" &amp; $N$1</f>
+        <v>'Menu-Superadmin'</v>
+      </c>
+      <c r="E297" t="str">
+        <f>$N$1 &amp; "Super Admin" &amp; $N$1</f>
+        <v>'Super Admin'</v>
+      </c>
+      <c r="F297" t="str">
+        <f t="shared" ref="F297:F310" si="34">"insert into sysLocalizationText Values(" &amp;A297 &amp; "," &amp; B297 &amp; "," &amp;C297 &amp; "," &amp; D297 &amp; "," &amp; E297 &amp; ",getdate(),getdate())"</f>
+        <v>insert into sysLocalizationText Values(1299,      'en-us','1299','Menu-Superadmin','Super Admin',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>1300</v>
+      </c>
+      <c r="B298" t="s">
+        <v>0</v>
+      </c>
+      <c r="C298" t="str">
+        <f t="shared" si="33"/>
+        <v>'1300'</v>
+      </c>
+      <c r="D298" t="str">
+        <f>$N$1 &amp; "Menu-Configs" &amp; $N$1</f>
+        <v>'Menu-Configs'</v>
+      </c>
+      <c r="E298" t="str">
+        <f>$N$1 &amp; "Business Configs" &amp; $N$1</f>
+        <v>'Business Configs'</v>
+      </c>
+      <c r="F298" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into sysLocalizationText Values(1300,      'en-us','1300','Menu-Configs','Business Configs',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>1301</v>
+      </c>
+      <c r="B299" t="s">
+        <v>0</v>
+      </c>
+      <c r="C299" t="str">
+        <f t="shared" si="33"/>
+        <v>'1301'</v>
+      </c>
+      <c r="D299" t="str">
+        <f>$N$1 &amp; "Menu-Instance" &amp; $N$1</f>
+        <v>'Menu-Instance'</v>
+      </c>
+      <c r="E299" t="str">
+        <f>$N$1 &amp; "Instances" &amp; $N$1</f>
+        <v>'Instances'</v>
+      </c>
+      <c r="F299" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into sysLocalizationText Values(1301,      'en-us','1301','Menu-Instance','Instances',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>1302</v>
+      </c>
+      <c r="B300" t="s">
+        <v>0</v>
+      </c>
+      <c r="C300" t="str">
+        <f t="shared" si="33"/>
+        <v>'1302'</v>
+      </c>
+      <c r="D300" t="str">
+        <f>$N$1 &amp; "Menu-Roles" &amp; $N$1</f>
+        <v>'Menu-Roles'</v>
+      </c>
+      <c r="E300" t="str">
+        <f>$N$1 &amp; "Roles" &amp; $N$1</f>
+        <v>'Roles'</v>
+      </c>
+      <c r="F300" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into sysLocalizationText Values(1302,      'en-us','1302','Menu-Roles','Roles',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>1303</v>
+      </c>
+      <c r="B301" t="s">
+        <v>0</v>
+      </c>
+      <c r="C301" t="str">
+        <f t="shared" si="33"/>
+        <v>'1303'</v>
+      </c>
+      <c r="D301" t="str">
+        <f>$N$1 &amp; "Menu-ObjectPermissions" &amp; $N$1</f>
+        <v>'Menu-ObjectPermissions'</v>
+      </c>
+      <c r="E301" t="str">
+        <f>$N$1 &amp; "Object Permissions" &amp; $N$1</f>
+        <v>'Object Permissions'</v>
+      </c>
+      <c r="F301" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into sysLocalizationText Values(1303,      'en-us','1303','Menu-ObjectPermissions','Object Permissions',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>1304</v>
+      </c>
+      <c r="B302" t="s">
+        <v>0</v>
+      </c>
+      <c r="C302" t="str">
+        <f t="shared" si="33"/>
+        <v>'1304'</v>
+      </c>
+      <c r="D302" t="str">
+        <f>$N$1 &amp; "Menu-Permissions" &amp; $N$1</f>
+        <v>'Menu-Permissions'</v>
+      </c>
+      <c r="E302" t="str">
+        <f>$N$1 &amp; "Permissions" &amp; $N$1</f>
+        <v>'Permissions'</v>
+      </c>
+      <c r="F302" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into sysLocalizationText Values(1304,      'en-us','1304','Menu-Permissions','Permissions',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>1305</v>
+      </c>
+      <c r="B303" t="s">
+        <v>0</v>
+      </c>
+      <c r="C303" t="str">
+        <f t="shared" si="33"/>
+        <v>'1305'</v>
+      </c>
+      <c r="D303" t="str">
+        <f>$N$1 &amp; "Menu-Users" &amp; $N$1</f>
+        <v>'Menu-Users'</v>
+      </c>
+      <c r="E303" t="str">
+        <f>$N$1 &amp; "Users" &amp; $N$1</f>
+        <v>'Users'</v>
+      </c>
+      <c r="F303" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into sysLocalizationText Values(1305,      'en-us','1305','Menu-Users','Users',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>1306</v>
+      </c>
+      <c r="B304" t="s">
+        <v>0</v>
+      </c>
+      <c r="C304" t="str">
+        <f t="shared" si="33"/>
+        <v>'1306'</v>
+      </c>
+      <c r="D304" t="str">
+        <f>$N$1 &amp; "Menu-LocalizationTexts" &amp; $N$1</f>
+        <v>'Menu-LocalizationTexts'</v>
+      </c>
+      <c r="E304" t="str">
+        <f>$N$1 &amp; "Localization Texts" &amp; $N$1</f>
+        <v>'Localization Texts'</v>
+      </c>
+      <c r="F304" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into sysLocalizationText Values(1306,      'en-us','1306','Menu-LocalizationTexts','Localization Texts',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>1307</v>
+      </c>
+      <c r="B305" t="s">
+        <v>0</v>
+      </c>
+      <c r="C305" t="str">
+        <f t="shared" si="33"/>
+        <v>'1307'</v>
+      </c>
+      <c r="D305" t="str">
+        <f>$N$1 &amp; "Menu-GroupParameters" &amp; $N$1</f>
+        <v>'Menu-GroupParameters'</v>
+      </c>
+      <c r="E305" t="str">
+        <f>$N$1 &amp; "Group Parameters" &amp; $N$1</f>
+        <v>'Group Parameters'</v>
+      </c>
+      <c r="F305" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into sysLocalizationText Values(1307,      'en-us','1307','Menu-GroupParameters','Group Parameters',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>1308</v>
+      </c>
+      <c r="B306" t="s">
+        <v>0</v>
+      </c>
+      <c r="C306" t="str">
+        <f t="shared" si="33"/>
+        <v>'1308'</v>
+      </c>
+      <c r="D306" t="str">
+        <f>$N$1 &amp; "Menu-Parameters" &amp; $N$1</f>
+        <v>'Menu-Parameters'</v>
+      </c>
+      <c r="E306" t="str">
+        <f>$N$1 &amp; "Parameters" &amp; $N$1</f>
+        <v>'Parameters'</v>
+      </c>
+      <c r="F306" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into sysLocalizationText Values(1308,      'en-us','1308','Menu-Parameters','Parameters',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>1309</v>
+      </c>
+      <c r="B307" t="s">
+        <v>0</v>
+      </c>
+      <c r="C307" t="str">
+        <f t="shared" si="33"/>
+        <v>'1309'</v>
+      </c>
+      <c r="D307" t="str">
+        <f>$N$1 &amp; "Menu-Monitoring" &amp; $N$1</f>
+        <v>'Menu-Monitoring'</v>
+      </c>
+      <c r="E307" t="str">
+        <f>$N$1 &amp; "Monitoring" &amp; $N$1</f>
+        <v>'Monitoring'</v>
+      </c>
+      <c r="F307" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into sysLocalizationText Values(1309,      'en-us','1309','Menu-Monitoring','Monitoring',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>1310</v>
+      </c>
+      <c r="B308" t="s">
+        <v>0</v>
+      </c>
+      <c r="C308" t="str">
+        <f t="shared" si="33"/>
+        <v>'1310'</v>
+      </c>
+      <c r="D308" t="str">
+        <f>$N$1 &amp; "Menu-SessionLog" &amp; $N$1</f>
+        <v>'Menu-SessionLog'</v>
+      </c>
+      <c r="E308" t="str">
+        <f>$N$1 &amp; "Session Log" &amp; $N$1</f>
+        <v>'Session Log'</v>
+      </c>
+      <c r="F308" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into sysLocalizationText Values(1310,      'en-us','1310','Menu-SessionLog','Session Log',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>1311</v>
+      </c>
+      <c r="B309" t="s">
+        <v>0</v>
+      </c>
+      <c r="C309" t="str">
+        <f t="shared" si="33"/>
+        <v>'1311'</v>
+      </c>
+      <c r="D309" t="str">
+        <f>$N$1 &amp; "Menu-DataLog" &amp; $N$1</f>
+        <v>'Menu-DataLog'</v>
+      </c>
+      <c r="E309" t="str">
+        <f>$N$1 &amp; "Data Log" &amp; $N$1</f>
+        <v>'Data Log'</v>
+      </c>
+      <c r="F309" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into sysLocalizationText Values(1311,      'en-us','1311','Menu-DataLog','Data Log',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>1312</v>
+      </c>
+      <c r="B310" t="s">
+        <v>0</v>
+      </c>
+      <c r="C310" t="str">
+        <f t="shared" si="33"/>
+        <v>'1312'</v>
+      </c>
+      <c r="D310" t="str">
+        <f>$N$1 &amp; "Menu-ExceptionLog" &amp; $N$1</f>
+        <v>'Menu-ExceptionLog'</v>
+      </c>
+      <c r="E310" t="str">
+        <f>$N$1 &amp; "Exception Log" &amp; $N$1</f>
+        <v>'Exception Log'</v>
+      </c>
+      <c r="F310" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into sysLocalizationText Values(1312,      'en-us','1312','Menu-ExceptionLog','Exception Log',getdate(),getdate())</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -7870,10 +8254,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N294"/>
+  <dimension ref="A1:N310"/>
   <sheetViews>
-    <sheetView topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="D284" sqref="D284"/>
+    <sheetView topLeftCell="E289" workbookViewId="0">
+      <selection activeCell="E301" sqref="E301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13976,7 +14360,7 @@
         <v>'Novo Grupo de Parâmetro'</v>
       </c>
       <c r="F258" t="str">
-        <f t="shared" ref="F258:F294" si="13">"insert into sysLocalizationText Values(" &amp;A258 &amp; "," &amp; B258 &amp; "," &amp;C258 &amp; "," &amp; D258 &amp; "," &amp; E258 &amp; ",getdate(),getdate())"</f>
+        <f t="shared" ref="F258:F310" si="13">"insert into sysLocalizationText Values(" &amp;A258 &amp; "," &amp; B258 &amp; "," &amp;C258 &amp; "," &amp; D258 &amp; "," &amp; E258 &amp; ",getdate(),getdate())"</f>
         <v>insert into sysLocalizationText Values(2260,      'pt-br','2260','NewGroupParameter-Label','Novo Grupo de Parâmetro',getdate(),getdate())</v>
       </c>
     </row>
@@ -14324,7 +14708,7 @@
         <v>97</v>
       </c>
       <c r="C273" t="str">
-        <f t="shared" ref="C273:C294" si="16">"'" &amp; A273 &amp; "'"</f>
+        <f t="shared" ref="C273:C296" si="16">"'" &amp; A273 &amp; "'"</f>
         <v>'2275'</v>
       </c>
       <c r="D273" t="str">
@@ -14838,6 +15222,390 @@
       <c r="F294" t="str">
         <f t="shared" si="13"/>
         <v>insert into sysLocalizationText Values(2296,      'pt-br','2296','Configs-PageTitle','Configurações',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>2297</v>
+      </c>
+      <c r="B295" t="s">
+        <v>97</v>
+      </c>
+      <c r="C295" t="str">
+        <f t="shared" si="16"/>
+        <v>'2297'</v>
+      </c>
+      <c r="D295" t="str">
+        <f>$N$1 &amp; "Logout-Label" &amp; $N$1</f>
+        <v>'Logout-Label'</v>
+      </c>
+      <c r="E295" t="str">
+        <f>$N$1 &amp; "Sair" &amp; $N$1</f>
+        <v>'Sair'</v>
+      </c>
+      <c r="F295" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2297,      'pt-br','2297','Logout-Label','Sair',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>2298</v>
+      </c>
+      <c r="B296" t="s">
+        <v>97</v>
+      </c>
+      <c r="C296" t="str">
+        <f t="shared" si="16"/>
+        <v>'2298'</v>
+      </c>
+      <c r="D296" t="str">
+        <f>$N$1 &amp; "AlterProfileImage-Description" &amp; $N$1</f>
+        <v>'AlterProfileImage-Description'</v>
+      </c>
+      <c r="E296" t="str">
+        <f>$N$1 &amp; "Arraste aqui o arquivo que deseja, ou clique no botão acima para navegar." &amp; $N$1</f>
+        <v>'Arraste aqui o arquivo que deseja, ou clique no botão acima para navegar.'</v>
+      </c>
+      <c r="F296" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2298,      'pt-br','2298','AlterProfileImage-Description','Arraste aqui o arquivo que deseja, ou clique no botão acima para navegar.',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>2299</v>
+      </c>
+      <c r="B297" t="s">
+        <v>97</v>
+      </c>
+      <c r="C297" t="str">
+        <f t="shared" ref="C297:C310" si="18">"'" &amp; A297 &amp; "'"</f>
+        <v>'2299'</v>
+      </c>
+      <c r="D297" t="str">
+        <f>$N$1 &amp; "Menu-Superadmin" &amp; $N$1</f>
+        <v>'Menu-Superadmin'</v>
+      </c>
+      <c r="E297" t="str">
+        <f>$N$1 &amp; "Super Admin" &amp; $N$1</f>
+        <v>'Super Admin'</v>
+      </c>
+      <c r="F297" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2299,      'pt-br','2299','Menu-Superadmin','Super Admin',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>2300</v>
+      </c>
+      <c r="B298" t="s">
+        <v>97</v>
+      </c>
+      <c r="C298" t="str">
+        <f t="shared" si="18"/>
+        <v>'2300'</v>
+      </c>
+      <c r="D298" t="str">
+        <f>$N$1 &amp; "Menu-Configs" &amp; $N$1</f>
+        <v>'Menu-Configs'</v>
+      </c>
+      <c r="E298" t="str">
+        <f>$N$1 &amp; "Configs de Negócio" &amp; $N$1</f>
+        <v>'Configs de Negócio'</v>
+      </c>
+      <c r="F298" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2300,      'pt-br','2300','Menu-Configs','Configs de Negócio',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>2301</v>
+      </c>
+      <c r="B299" t="s">
+        <v>97</v>
+      </c>
+      <c r="C299" t="str">
+        <f t="shared" si="18"/>
+        <v>'2301'</v>
+      </c>
+      <c r="D299" t="str">
+        <f>$N$1 &amp; "Menu-Instance" &amp; $N$1</f>
+        <v>'Menu-Instance'</v>
+      </c>
+      <c r="E299" t="str">
+        <f>$N$1 &amp; "Instâncias" &amp; $N$1</f>
+        <v>'Instâncias'</v>
+      </c>
+      <c r="F299" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2301,      'pt-br','2301','Menu-Instance','Instâncias',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>2302</v>
+      </c>
+      <c r="B300" t="s">
+        <v>97</v>
+      </c>
+      <c r="C300" t="str">
+        <f t="shared" si="18"/>
+        <v>'2302'</v>
+      </c>
+      <c r="D300" t="str">
+        <f>$N$1 &amp; "Menu-Roles" &amp; $N$1</f>
+        <v>'Menu-Roles'</v>
+      </c>
+      <c r="E300" t="str">
+        <f>$N$1 &amp; "Roles" &amp; $N$1</f>
+        <v>'Roles'</v>
+      </c>
+      <c r="F300" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2302,      'pt-br','2302','Menu-Roles','Roles',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>2303</v>
+      </c>
+      <c r="B301" t="s">
+        <v>97</v>
+      </c>
+      <c r="C301" t="str">
+        <f t="shared" si="18"/>
+        <v>'2303'</v>
+      </c>
+      <c r="D301" t="str">
+        <f>$N$1 &amp; "Menu-ObjectPermissions" &amp; $N$1</f>
+        <v>'Menu-ObjectPermissions'</v>
+      </c>
+      <c r="E301" t="str">
+        <f>$N$1 &amp; "Objetos de Permissões" &amp; $N$1</f>
+        <v>'Objetos de Permissões'</v>
+      </c>
+      <c r="F301" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2303,      'pt-br','2303','Menu-ObjectPermissions','Objetos de Permissões',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>2304</v>
+      </c>
+      <c r="B302" t="s">
+        <v>97</v>
+      </c>
+      <c r="C302" t="str">
+        <f t="shared" si="18"/>
+        <v>'2304'</v>
+      </c>
+      <c r="D302" t="str">
+        <f>$N$1 &amp; "Menu-Permissions" &amp; $N$1</f>
+        <v>'Menu-Permissions'</v>
+      </c>
+      <c r="E302" t="str">
+        <f>$N$1 &amp; "Permissões" &amp; $N$1</f>
+        <v>'Permissões'</v>
+      </c>
+      <c r="F302" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2304,      'pt-br','2304','Menu-Permissions','Permissões',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>2305</v>
+      </c>
+      <c r="B303" t="s">
+        <v>97</v>
+      </c>
+      <c r="C303" t="str">
+        <f t="shared" si="18"/>
+        <v>'2305'</v>
+      </c>
+      <c r="D303" t="str">
+        <f>$N$1 &amp; "Menu-Users" &amp; $N$1</f>
+        <v>'Menu-Users'</v>
+      </c>
+      <c r="E303" t="str">
+        <f>$N$1 &amp; "Usuários" &amp; $N$1</f>
+        <v>'Usuários'</v>
+      </c>
+      <c r="F303" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2305,      'pt-br','2305','Menu-Users','Usuários',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>2306</v>
+      </c>
+      <c r="B304" t="s">
+        <v>97</v>
+      </c>
+      <c r="C304" t="str">
+        <f t="shared" si="18"/>
+        <v>'2306'</v>
+      </c>
+      <c r="D304" t="str">
+        <f>$N$1 &amp; "Menu-LocalizationTexts" &amp; $N$1</f>
+        <v>'Menu-LocalizationTexts'</v>
+      </c>
+      <c r="E304" t="str">
+        <f>$N$1 &amp; "Textos de Localização" &amp; $N$1</f>
+        <v>'Textos de Localização'</v>
+      </c>
+      <c r="F304" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2306,      'pt-br','2306','Menu-LocalizationTexts','Textos de Localização',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>2307</v>
+      </c>
+      <c r="B305" t="s">
+        <v>97</v>
+      </c>
+      <c r="C305" t="str">
+        <f t="shared" si="18"/>
+        <v>'2307'</v>
+      </c>
+      <c r="D305" t="str">
+        <f>$N$1 &amp; "Menu-GroupParameters" &amp; $N$1</f>
+        <v>'Menu-GroupParameters'</v>
+      </c>
+      <c r="E305" t="str">
+        <f>$N$1 &amp; "Grupo de Parâmetros" &amp; $N$1</f>
+        <v>'Grupo de Parâmetros'</v>
+      </c>
+      <c r="F305" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2307,      'pt-br','2307','Menu-GroupParameters','Grupo de Parâmetros',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>2308</v>
+      </c>
+      <c r="B306" t="s">
+        <v>97</v>
+      </c>
+      <c r="C306" t="str">
+        <f t="shared" si="18"/>
+        <v>'2308'</v>
+      </c>
+      <c r="D306" t="str">
+        <f>$N$1 &amp; "Menu-Parameters" &amp; $N$1</f>
+        <v>'Menu-Parameters'</v>
+      </c>
+      <c r="E306" t="str">
+        <f>$N$1 &amp; "Parâmetros" &amp; $N$1</f>
+        <v>'Parâmetros'</v>
+      </c>
+      <c r="F306" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2308,      'pt-br','2308','Menu-Parameters','Parâmetros',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>2309</v>
+      </c>
+      <c r="B307" t="s">
+        <v>97</v>
+      </c>
+      <c r="C307" t="str">
+        <f t="shared" si="18"/>
+        <v>'2309'</v>
+      </c>
+      <c r="D307" t="str">
+        <f>$N$1 &amp; "Menu-Monitoring" &amp; $N$1</f>
+        <v>'Menu-Monitoring'</v>
+      </c>
+      <c r="E307" t="str">
+        <f>$N$1 &amp; "Monitoramento" &amp; $N$1</f>
+        <v>'Monitoramento'</v>
+      </c>
+      <c r="F307" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2309,      'pt-br','2309','Menu-Monitoring','Monitoramento',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>2310</v>
+      </c>
+      <c r="B308" t="s">
+        <v>97</v>
+      </c>
+      <c r="C308" t="str">
+        <f t="shared" si="18"/>
+        <v>'2310'</v>
+      </c>
+      <c r="D308" t="str">
+        <f>$N$1 &amp; "Menu-SessionLog" &amp; $N$1</f>
+        <v>'Menu-SessionLog'</v>
+      </c>
+      <c r="E308" t="str">
+        <f>$N$1 &amp; "Logs de Acessos" &amp; $N$1</f>
+        <v>'Logs de Acessos'</v>
+      </c>
+      <c r="F308" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2310,      'pt-br','2310','Menu-SessionLog','Logs de Acessos',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>2311</v>
+      </c>
+      <c r="B309" t="s">
+        <v>97</v>
+      </c>
+      <c r="C309" t="str">
+        <f t="shared" si="18"/>
+        <v>'2311'</v>
+      </c>
+      <c r="D309" t="str">
+        <f>$N$1 &amp; "Menu-DataLog" &amp; $N$1</f>
+        <v>'Menu-DataLog'</v>
+      </c>
+      <c r="E309" t="str">
+        <f>$N$1 &amp; "Logs de Dados" &amp; $N$1</f>
+        <v>'Logs de Dados'</v>
+      </c>
+      <c r="F309" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2311,      'pt-br','2311','Menu-DataLog','Logs de Dados',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>2312</v>
+      </c>
+      <c r="B310" t="s">
+        <v>97</v>
+      </c>
+      <c r="C310" t="str">
+        <f t="shared" si="18"/>
+        <v>'2312'</v>
+      </c>
+      <c r="D310" t="str">
+        <f>$N$1 &amp; "Menu-ExceptionLog" &amp; $N$1</f>
+        <v>'Menu-ExceptionLog'</v>
+      </c>
+      <c r="E310" t="str">
+        <f>$N$1 &amp; "Logs de Erros" &amp; $N$1</f>
+        <v>'Logs de Erros'</v>
+      </c>
+      <c r="F310" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2312,      'pt-br','2312','Menu-ExceptionLog','Logs de Erros',getdate(),getdate())</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continuação do desenvolvimento da V2.
Implementação da página de ExceptionsLog.
</commit_message>
<xml_diff>
--- a/Docs/InsertLocalizationText.xlsx
+++ b/Docs/InsertLocalizationText.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="156">
   <si>
     <t xml:space="preserve">      'en-us'</t>
   </si>
@@ -884,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N317"/>
+  <dimension ref="A1:N320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="F315" sqref="F315:F317"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2789,12 +2789,12 @@
         <v>'LoginTitle-Description'</v>
       </c>
       <c r="E83" t="str">
-        <f>$N$1 &amp; "Enter your login and password" &amp; $N$1</f>
-        <v>'Enter your login and password'</v>
+        <f>$N$1 &amp; "Enter your access credentials" &amp; $N$1</f>
+        <v>'Enter your access credentials'</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="3"/>
-        <v>insert into sysLocalizationText Values(1083,      'en-us','1083','LoginTitle-Description','Enter your login and password',getdate(),getdate())</v>
+        <v>insert into sysLocalizationText Values(1083,      'en-us','1083','LoginTitle-Description','Enter your access credentials',getdate(),getdate())</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -8397,7 +8397,7 @@
         <v>0</v>
       </c>
       <c r="C317" t="str">
-        <f t="shared" ref="C317" si="44">"'" &amp; A317 &amp; "'"</f>
+        <f t="shared" ref="C317:C318" si="44">"'" &amp; A317 &amp; "'"</f>
         <v>'1319'</v>
       </c>
       <c r="D317" t="str">
@@ -8409,8 +8409,80 @@
         <v>'Delete'</v>
       </c>
       <c r="F317" t="str">
-        <f t="shared" ref="F317" si="45">"insert into sysLocalizationText Values(" &amp;A317 &amp; "," &amp; B317 &amp; "," &amp;C317 &amp; "," &amp; D317 &amp; "," &amp; E317 &amp; ",getdate(),getdate())"</f>
+        <f t="shared" ref="F317:F318" si="45">"insert into sysLocalizationText Values(" &amp;A317 &amp; "," &amp; B317 &amp; "," &amp;C317 &amp; "," &amp; D317 &amp; "," &amp; E317 &amp; ",getdate(),getdate())"</f>
         <v>insert into sysLocalizationText Values(1319,      'en-us','1319','AllowDelete-Label','Delete',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>1320</v>
+      </c>
+      <c r="B318" t="s">
+        <v>0</v>
+      </c>
+      <c r="C318" t="str">
+        <f t="shared" si="44"/>
+        <v>'1320'</v>
+      </c>
+      <c r="D318" t="str">
+        <f>$N$1 &amp; "InsertOperation-Text" &amp; $N$1</f>
+        <v>'InsertOperation-Text'</v>
+      </c>
+      <c r="E318" t="str">
+        <f>$N$1 &amp; "Insert" &amp; $N$1</f>
+        <v>'Insert'</v>
+      </c>
+      <c r="F318" t="str">
+        <f t="shared" si="45"/>
+        <v>insert into sysLocalizationText Values(1320,      'en-us','1320','InsertOperation-Text','Insert',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>1321</v>
+      </c>
+      <c r="B319" t="s">
+        <v>0</v>
+      </c>
+      <c r="C319" t="str">
+        <f t="shared" ref="C319:C320" si="46">"'" &amp; A319 &amp; "'"</f>
+        <v>'1321'</v>
+      </c>
+      <c r="D319" t="str">
+        <f>$N$1 &amp; "UpdateOperation-Text" &amp; $N$1</f>
+        <v>'UpdateOperation-Text'</v>
+      </c>
+      <c r="E319" t="str">
+        <f>$N$1 &amp; "Update" &amp; $N$1</f>
+        <v>'Update'</v>
+      </c>
+      <c r="F319" t="str">
+        <f t="shared" ref="F319:F320" si="47">"insert into sysLocalizationText Values(" &amp;A319 &amp; "," &amp; B319 &amp; "," &amp;C319 &amp; "," &amp; D319 &amp; "," &amp; E319 &amp; ",getdate(),getdate())"</f>
+        <v>insert into sysLocalizationText Values(1321,      'en-us','1321','UpdateOperation-Text','Update',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>1322</v>
+      </c>
+      <c r="B320" t="s">
+        <v>0</v>
+      </c>
+      <c r="C320" t="str">
+        <f t="shared" si="46"/>
+        <v>'1322'</v>
+      </c>
+      <c r="D320" t="str">
+        <f>$N$1 &amp; "DeleteOperation-Text" &amp; $N$1</f>
+        <v>'DeleteOperation-Text'</v>
+      </c>
+      <c r="E320" t="str">
+        <f>$N$1 &amp; "Delete" &amp; $N$1</f>
+        <v>'Delete'</v>
+      </c>
+      <c r="F320" t="str">
+        <f t="shared" si="47"/>
+        <v>insert into sysLocalizationText Values(1322,      'en-us','1322','DeleteOperation-Text','Delete',getdate(),getdate())</v>
       </c>
     </row>
   </sheetData>
@@ -8422,10 +8494,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N317"/>
+  <dimension ref="A1:N320"/>
   <sheetViews>
-    <sheetView topLeftCell="A288" workbookViewId="0">
-      <selection activeCell="F315" sqref="F315:F317"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10324,12 +10396,12 @@
         <v>'LoginTitle-Description'</v>
       </c>
       <c r="E83" t="str">
-        <f>$N$1 &amp; "Insira seu login e senha" &amp; $N$1</f>
-        <v>'Insira seu login e senha'</v>
+        <f>$N$1 &amp; "Insira suas credenciais de acesso" &amp; $N$1</f>
+        <v>'Insira suas credenciais de acesso'</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="3"/>
-        <v>insert into sysLocalizationText Values(2083,      'pt-br','2083','LoginTitle-Description','Insira seu login e senha',getdate(),getdate())</v>
+        <v>insert into sysLocalizationText Values(2083,      'pt-br','2083','LoginTitle-Description','Insira suas credenciais de acesso',getdate(),getdate())</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -14528,7 +14600,7 @@
         <v>'Novo Grupo de Parâmetro'</v>
       </c>
       <c r="F258" t="str">
-        <f t="shared" ref="F258:F317" si="13">"insert into sysLocalizationText Values(" &amp;A258 &amp; "," &amp; B258 &amp; "," &amp;C258 &amp; "," &amp; D258 &amp; "," &amp; E258 &amp; ",getdate(),getdate())"</f>
+        <f t="shared" ref="F258:F320" si="13">"insert into sysLocalizationText Values(" &amp;A258 &amp; "," &amp; B258 &amp; "," &amp;C258 &amp; "," &amp; D258 &amp; "," &amp; E258 &amp; ",getdate(),getdate())"</f>
         <v>insert into sysLocalizationText Values(2260,      'pt-br','2260','NewGroupParameter-Label','Novo Grupo de Parâmetro',getdate(),getdate())</v>
       </c>
     </row>
@@ -15448,7 +15520,7 @@
         <v>97</v>
       </c>
       <c r="C297" t="str">
-        <f t="shared" ref="C297:C317" si="18">"'" &amp; A297 &amp; "'"</f>
+        <f t="shared" ref="C297:C320" si="18">"'" &amp; A297 &amp; "'"</f>
         <v>'2299'</v>
       </c>
       <c r="D297" t="str">
@@ -15942,6 +16014,78 @@
       <c r="F317" t="str">
         <f t="shared" si="13"/>
         <v>insert into sysLocalizationText Values(2319,      'pt-br','2319','AllowDelete-Label','Remover',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>2320</v>
+      </c>
+      <c r="B318" t="s">
+        <v>97</v>
+      </c>
+      <c r="C318" t="str">
+        <f t="shared" si="18"/>
+        <v>'2320'</v>
+      </c>
+      <c r="D318" t="str">
+        <f>$N$1 &amp; "InsertOperation-Text" &amp; $N$1</f>
+        <v>'InsertOperation-Text'</v>
+      </c>
+      <c r="E318" t="str">
+        <f>$N$1 &amp; "Inserção" &amp; $N$1</f>
+        <v>'Inserção'</v>
+      </c>
+      <c r="F318" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2320,      'pt-br','2320','InsertOperation-Text','Inserção',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>2321</v>
+      </c>
+      <c r="B319" t="s">
+        <v>97</v>
+      </c>
+      <c r="C319" t="str">
+        <f t="shared" si="18"/>
+        <v>'2321'</v>
+      </c>
+      <c r="D319" t="str">
+        <f>$N$1 &amp; "UpdateOperation-Text" &amp; $N$1</f>
+        <v>'UpdateOperation-Text'</v>
+      </c>
+      <c r="E319" t="str">
+        <f>$N$1 &amp; "Edição" &amp; $N$1</f>
+        <v>'Edição'</v>
+      </c>
+      <c r="F319" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2321,      'pt-br','2321','UpdateOperation-Text','Edição',getdate(),getdate())</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>2322</v>
+      </c>
+      <c r="B320" t="s">
+        <v>97</v>
+      </c>
+      <c r="C320" t="str">
+        <f t="shared" si="18"/>
+        <v>'2322'</v>
+      </c>
+      <c r="D320" t="str">
+        <f>$N$1 &amp; "DeleteOperation-Text" &amp; $N$1</f>
+        <v>'DeleteOperation-Text'</v>
+      </c>
+      <c r="E320" t="str">
+        <f>$N$1 &amp; "Exclusão" &amp; $N$1</f>
+        <v>'Exclusão'</v>
+      </c>
+      <c r="F320" t="str">
+        <f t="shared" si="13"/>
+        <v>insert into sysLocalizationText Values(2322,      'pt-br','2322','DeleteOperation-Text','Exclusão',getdate(),getdate())</v>
       </c>
     </row>
   </sheetData>

</xml_diff>